<commit_message>
Added click to UIBank_Login to accept privacy policy
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8704ae8fe955a777/Documents/UiPath/UiBank-Account-Transaction-Compilation-Export/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DevilsDice\Desktop\CourseStuff\Traineeship\UIPath Development\UIPath Workspace\UiBankAccountTransactionCompilationAndExport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{4F43AFA8-96E9-4359-97F0-A8428858A95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{952F3407-5BDB-4641-A29E-8B60D8BC5BF9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF7E7619-6FA0-4465-A3C2-3DE2AB446523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="27150" yWindow="4410" windowWidth="26850" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="49">
   <si>
     <t>Name</t>
   </si>
@@ -165,6 +165,12 @@
   </si>
   <si>
     <t>https://uibank.uipath.com/welcome</t>
+  </si>
+  <si>
+    <t>UiBank_Accounts_URL</t>
+  </si>
+  <si>
+    <t>https://uibank.uipath.com/accounts</t>
   </si>
 </sst>
 </file>
@@ -552,15 +558,15 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5546875" customWidth="1"/>
-    <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="81.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -611,7 +617,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="43.2">
+    <row r="4" spans="1:26" ht="45">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -621,7 +627,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="6" spans="1:26" ht="28.8">
+    <row r="6" spans="1:26" ht="30">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -641,7 +647,14 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1635,9 +1648,10 @@
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" xr:uid="{9B5F029C-C9CB-4B36-9A7E-DEB9DA22714E}"/>
+    <hyperlink ref="B9" r:id="rId2" xr:uid="{E54D040C-CD05-4DF4-A92C-6CED3773A7C8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1649,12 +1663,12 @@
       <selection activeCell="A19" sqref="A18:XFD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.44140625" customWidth="1"/>
-    <col min="4" max="26" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="75.42578125" customWidth="1"/>
+    <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1691,7 +1705,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="28.8">
+    <row r="2" spans="1:26" ht="30">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1702,7 +1716,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="43.2">
+    <row r="3" spans="1:26" ht="45">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -1816,7 +1830,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="28.8">
+    <row r="17" spans="1:3" ht="45">
       <c r="A17" t="s">
         <v>38</v>
       </c>
@@ -2808,12 +2822,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.88671875" customWidth="1"/>
-    <col min="2" max="2" width="30.109375" customWidth="1"/>
-    <col min="3" max="3" width="60.33203125" customWidth="1"/>
-    <col min="4" max="26" width="65.44140625" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
+    <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
updated the main, merge and login with changes from jamie branch
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DevilsDice\Desktop\CourseStuff\Traineeship\UIPath Development\UIPath Workspace\UiBankAccountTransactionCompilationAndExport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F0BBF8-A570-4BBB-BA72-451732BC41DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79247B32-353E-438F-94AB-2BC0A60C4407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38580" yWindow="3870" windowWidth="26850" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45900" yWindow="2805" windowWidth="26850" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -161,9 +161,6 @@
     <t>UiBank Account Transaction Compilation &amp; Export</t>
   </si>
   <si>
-    <t>URL</t>
-  </si>
-  <si>
     <t>https://uibank.uipath.com/welcome</t>
   </si>
   <si>
@@ -198,6 +195,15 @@
   </si>
   <si>
     <t>The body of the email that will be sent</t>
+  </si>
+  <si>
+    <t>UiBank_Login_URL</t>
+  </si>
+  <si>
+    <t>C:\temp\TransactionHistory\</t>
+  </si>
+  <si>
+    <t>Temp_TransactionsHistory_Folder_Path</t>
   </si>
 </sst>
 </file>
@@ -585,13 +591,13 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="87.42578125" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -668,56 +674,63 @@
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>47</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="32.25" customHeight="1">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
Added UIBank Credentials to Config
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DevilsDice\Desktop\CourseStuff\Traineeship\UIPath Development\UIPath Workspace\UiBankAccountTransactionCompilationAndExport\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79247B32-353E-438F-94AB-2BC0A60C4407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09ED8A5A-29D8-454A-BD08-207EC6DB6157}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45900" yWindow="2805" windowWidth="26850" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52845" yWindow="1110" windowWidth="18795" windowHeight="16200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -204,6 +204,12 @@
   </si>
   <si>
     <t>Temp_TransactionsHistory_Folder_Path</t>
+  </si>
+  <si>
+    <t>UiBank_Credentials</t>
+  </si>
+  <si>
+    <t>UiBankCredentials</t>
   </si>
 </sst>
 </file>
@@ -588,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -688,66 +694,75 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B10" s="5"/>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A12" t="s">
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
         <v>50</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>52</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="32.25" customHeight="1">
-      <c r="A13" t="s">
+    <row r="15" spans="1:26" ht="32.25" customHeight="1">
+      <c r="A15" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B15" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1714,12 +1729,14 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" xr:uid="{9B5F029C-C9CB-4B36-9A7E-DEB9DA22714E}"/>
     <hyperlink ref="B9" r:id="rId2" xr:uid="{E54D040C-CD05-4DF4-A92C-6CED3773A7C8}"/>
-    <hyperlink ref="B11" r:id="rId3" xr:uid="{4CA8E156-4628-4611-BD43-1DC877B37FF4}"/>
+    <hyperlink ref="B13" r:id="rId3" xr:uid="{4CA8E156-4628-4611-BD43-1DC877B37FF4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>

</xml_diff>